<commit_message>
refactoring: Updating TPI files guide
</commit_message>
<xml_diff>
--- a/public/tpi/export_support/User guide TPI files.xlsx
+++ b/public/tpi/export_support/User guide TPI files.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
   <si>
     <r>
       <rPr>
@@ -453,7 +453,7 @@
     <t>CP Publication Date</t>
   </si>
   <si>
-    <t>Date on which the company's Carbon Performance assessment was published on the website (companies are assessed annually)</t>
+    <t>Date on which the company's Carbon Performance assessment was conducted (companies are assessed annually). Please note the Carbon Performance data for CA100+ companies is released at a later date compared to other companies assessed by TPI. Therefore, non-CA100 companies within each sector may display more up-to-date publication dates until quarter three of a given year. By quarter three, data for all companies, including CA100+ companies will have been published, completing the annual assessment cycle.</t>
   </si>
   <si>
     <t>AG</t>
@@ -554,6 +554,25 @@
   </si>
   <si>
     <t>A variable showing the company's alignment with the benchmarks in 2027 during the previous Carbon Performance assessment</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">*Note that TPI has only started disclosing company's alignment in 2027 in 2024 hence </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>this column should be blank as of January 2022</t>
+    </r>
   </si>
   <si>
     <t>AN</t>
@@ -770,7 +789,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -797,28 +816,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -827,16 +846,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="medium">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -882,22 +901,22 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
@@ -1055,73 +1074,73 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1150,10 +1169,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffe1ff"/>
       <rgbColor rgb="ffb4c6e7"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1352,17 +1371,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1389,10 +1408,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1631,12 +1650,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1913,7 +1932,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1940,10 +1959,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3170,7 +3189,7 @@
       <c r="AT17" s="2"/>
       <c r="AU17" s="2"/>
     </row>
-    <row r="18" ht="28.8" customHeight="1">
+    <row r="18" ht="71.05" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" t="s" s="13">
         <v>55</v>
@@ -3717,7 +3736,7 @@
         <v>85</v>
       </c>
       <c r="E27" t="s" s="15">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F27" t="s" s="15">
         <v>9</v>
@@ -3767,13 +3786,13 @@
     <row r="28" ht="28.8" customHeight="1">
       <c r="A28" s="4"/>
       <c r="B28" t="s" s="13">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s" s="14">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s" s="15">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s" s="15">
         <v>83</v>
@@ -3826,13 +3845,13 @@
     <row r="29" ht="28.8" customHeight="1">
       <c r="A29" s="4"/>
       <c r="B29" t="s" s="13">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s" s="14">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s" s="15">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E29" s="16"/>
       <c r="F29" t="s" s="15">
@@ -3883,16 +3902,16 @@
     <row r="30" ht="28.8" customHeight="1">
       <c r="A30" s="4"/>
       <c r="B30" t="s" s="13">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s" s="14">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D30" t="s" s="15">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E30" t="s" s="15">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s" s="15">
         <v>9</v>
@@ -3942,13 +3961,13 @@
     <row r="31" ht="28.8" customHeight="1">
       <c r="A31" s="4"/>
       <c r="B31" t="s" s="13">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s" s="14">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D31" t="s" s="15">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E31" s="16"/>
       <c r="F31" t="s" s="15">
@@ -3999,13 +4018,13 @@
     <row r="32" ht="13.55" customHeight="1">
       <c r="A32" s="4"/>
       <c r="B32" t="s" s="13">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C32" t="s" s="14">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D32" t="s" s="15">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E32" s="16"/>
       <c r="F32" t="s" s="15">
@@ -4056,17 +4075,17 @@
     <row r="33" ht="28.8" customHeight="1">
       <c r="A33" s="4"/>
       <c r="B33" t="s" s="13">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s" s="14">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D33" t="s" s="15">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E33" s="16"/>
       <c r="F33" t="s" s="15">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G33" s="17"/>
       <c r="H33" s="8"/>
@@ -4113,13 +4132,13 @@
     <row r="34" ht="31.5" customHeight="1">
       <c r="A34" s="4"/>
       <c r="B34" t="s" s="20">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s" s="21">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D34" t="s" s="22">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E34" s="23"/>
       <c r="F34" t="s" s="22">
@@ -4869,13 +4888,13 @@
       <c r="AT12" s="2"/>
       <c r="AU12" s="2"/>
     </row>
-    <row r="13" ht="28.8" customHeight="1">
+    <row r="13" ht="65.55" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" t="s" s="13">
         <v>34</v>
       </c>
       <c r="C13" t="s" s="14">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D13" t="s" s="15">
         <v>57</v>
@@ -4934,7 +4953,7 @@
         <v>38</v>
       </c>
       <c r="C14" t="s" s="14">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D14" t="s" s="15">
         <v>60</v>
@@ -5175,7 +5194,7 @@
     <row r="18" ht="28.8" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" t="s" s="13">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C18" t="s" s="14">
         <v>75</v>
@@ -5236,7 +5255,7 @@
     <row r="19" ht="13.55" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" t="s" s="13">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s" s="14">
         <v>78</v>
@@ -5293,7 +5312,7 @@
     <row r="20" ht="28.8" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" t="s" s="13">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s" s="14">
         <v>62</v>
@@ -5350,13 +5369,13 @@
     <row r="21" ht="28.8" customHeight="1">
       <c r="A21" s="4"/>
       <c r="B21" t="s" s="13">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s" s="14">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D21" t="s" s="15">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" t="s" s="15">
@@ -5407,13 +5426,13 @@
     <row r="22" ht="13.55" customHeight="1">
       <c r="A22" s="4"/>
       <c r="B22" t="s" s="13">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s" s="14">
         <v>41</v>
       </c>
       <c r="D22" t="s" s="15">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" t="s" s="15">
@@ -5464,13 +5483,13 @@
     <row r="23" ht="13.55" customHeight="1">
       <c r="A23" s="4"/>
       <c r="B23" t="s" s="13">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C23" t="s" s="14">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D23" t="s" s="15">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E23" s="16"/>
       <c r="F23" t="s" s="15">
@@ -5521,17 +5540,17 @@
     <row r="24" ht="29.4" customHeight="1">
       <c r="A24" s="4"/>
       <c r="B24" t="s" s="20">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C24" t="s" s="21">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D24" t="s" s="22">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E24" s="23"/>
       <c r="F24" t="s" s="22">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G24" s="24"/>
       <c r="H24" s="8"/>
@@ -6049,7 +6068,7 @@
         <v>19</v>
       </c>
       <c r="C9" t="s" s="14">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s" s="15">
         <v>21</v>
@@ -6283,7 +6302,7 @@
         <v>34</v>
       </c>
       <c r="C13" t="s" s="14">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D13" t="s" s="15">
         <v>36</v>
@@ -6342,7 +6361,7 @@
         <v>38</v>
       </c>
       <c r="C14" t="s" s="14">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D14" t="s" s="15">
         <v>40</v>
@@ -6462,7 +6481,7 @@
         <v>47</v>
       </c>
       <c r="C16" t="s" s="14">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D16" t="s" s="15">
         <v>49</v>
@@ -6521,13 +6540,13 @@
         <v>51</v>
       </c>
       <c r="C17" t="s" s="21">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D17" t="s" s="22">
         <v>53</v>
       </c>
       <c r="E17" t="s" s="22">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F17" t="s" s="22">
         <v>9</v>
@@ -6665,7 +6684,7 @@
         <v>63</v>
       </c>
       <c r="E5" t="s" s="15">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F5" t="s" s="15">
         <v>9</v>
@@ -6678,7 +6697,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s" s="14">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D6" t="s" s="15">
         <v>18</v>
@@ -6695,13 +6714,13 @@
         <v>13</v>
       </c>
       <c r="C7" t="s" s="14">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D7" t="s" s="15">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s" s="15">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F7" t="s" s="15">
         <v>9</v>
@@ -6716,10 +6735,10 @@
         <v>16</v>
       </c>
       <c r="C8" t="s" s="14">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D8" t="s" s="15">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E8" t="s" s="15">
         <v>37</v>
@@ -6735,10 +6754,10 @@
         <v>19</v>
       </c>
       <c r="C9" t="s" s="14">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D9" t="s" s="15">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" t="s" s="15">
@@ -6749,17 +6768,17 @@
     <row r="10" ht="15" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" t="s" s="20">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s" s="21">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s" s="22">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" t="s" s="22">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G10" s="24"/>
     </row>

</xml_diff>

<commit_message>
refactoring: Update of TPI user guides file
</commit_message>
<xml_diff>
--- a/public/tpi/export_support/User guide TPI files.xlsx
+++ b/public/tpi/export_support/User guide TPI files.xlsx
@@ -1,26 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMINA3\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271ADB1A-B113-4AF4-BC3A-1BBCE84C730D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Company_Latest_Assessments.csv" sheetId="1" r:id="rId4"/>
-    <sheet name="CP_Assessments_(date).csv" sheetId="2" r:id="rId5"/>
-    <sheet name="MQ_Assessments_Methodology.csv" sheetId="3" r:id="rId6"/>
-    <sheet name="Sectoral_Benchmarks_(date).csv" sheetId="4" r:id="rId7"/>
+    <sheet name="Company_Latest_Assessments.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="CP_Assessments_(date).csv" sheetId="2" r:id="rId2"/>
+    <sheet name="MQ_Assessments_Methodology.csv" sheetId="3" r:id="rId3"/>
+    <sheet name="Sectoral_Benchmarks_(date).csv" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="135">
   <si>
     <r>
       <rPr>
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">TPI’s full historical dataset is available on our website: https://transitionpathwayinitiative.org/sectors. If you click “Download all sector data”, you will download a zipped folder. Please also consult TPI's methodology report and sectoral methodology notes when interpreting TPI data. All TPI publication are available on our website: https://www.transitionpathwayinitiative.org/publications.
 </t>
@@ -30,17 +53,19 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
-        <u val="single"/>
+        <b/>
+        <u/>
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Latest MQ and CP Assessments:</t>
     </r>
@@ -49,6 +74,7 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -58,16 +84,18 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">The latest assessments of both Management Quality and Carbon Performance can be found in the </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
-        <u val="single"/>
+        <b/>
+        <u/>
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Company_Latest_Assessments file</t>
     </r>
@@ -76,6 +104,7 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">. This file allows comparisons between companies' previous and current scores.
 </t>
@@ -85,17 +114,19 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
-        <u val="single"/>
+        <b/>
+        <u/>
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Management Quality Assessments:
 </t>
@@ -105,16 +136,18 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">All published assessments can be found in: </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
-        <u val="single"/>
+        <b/>
+        <u/>
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>MQ_Assessments_Methodology_1-4_xxxxx</t>
     </r>
@@ -123,6 +156,7 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (note that the last digits provide the date on which the dataset was downloaded by the website user)
 </t>
@@ -132,6 +166,7 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">• The MQ_Assessments_Methodology_1 file refers to TPI’s first research cycle: it contains assessments conducted in 2015-2017 (see the Assessment Date column for each company) and published on TPI’s website in 2017-2018 (see the Publication Date column for each company). 
 </t>
@@ -141,6 +176,7 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">• Methodology 2 contains assessments conducted in the following period (2017-2018) and published in 2018-2019. 
 </t>
@@ -150,6 +186,7 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">• Methodology 3 contains two assessment cycles: (1) assessments conducted in 2018-2019 and published in 2019-2020 and (2) assessments conducted in 2019-2020 and published in 2020 and early 2021. 
 </t>
@@ -159,6 +196,7 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">• Methodology 4 our assessments conducted in 2020-2021 and published in 2021.
 </t>
@@ -168,6 +206,7 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">*Our assessment cycles were not organised on a strict calendar year basis. The column called Assessment Date enables the website user to organise the assessment data for each company chronologically.
 </t>
@@ -177,17 +216,19 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
-        <u val="single"/>
+        <b/>
+        <u/>
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Carbon Performance Assessments:
 </t>
@@ -197,16 +238,18 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">All assessment data and alignment scores are provided in the Excel workbook </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
-        <u val="single"/>
+        <b/>
+        <u/>
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>CP_Assessments_xxxx</t>
     </r>
@@ -215,6 +258,7 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">. For every company, assessments appear in separate rows per research cycle. Note that new companies were added to the TPI universe each year, so not all companies have been assessed over the full 2017-(current year) period.
 </t>
@@ -224,17 +268,19 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
-        <u val="single"/>
+        <b/>
+        <u/>
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Benchmarks:</t>
     </r>
@@ -243,6 +289,7 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -252,25 +299,28 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>All TPI’s sectoral benchmarks for carbon performance assessments are provided in the Excel workbook</t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
-        <u val="single"/>
+        <b/>
+        <u/>
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Sectoral_benchmark_xxxx</t>
     </r>
@@ -279,6 +329,7 @@
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">.
 </t>
@@ -453,9 +504,6 @@
     <t>CP Publication Date</t>
   </si>
   <si>
-    <t>Date on which the company's Carbon Performance assessment was conducted (companies are assessed annually). Please note the Carbon Performance data for CA100+ companies is released at a later date compared to other companies assessed by TPI. Therefore, non-CA100 companies within each sector may display more up-to-date publication dates until quarter three of a given year. By quarter three, data for all companies, including CA100+ companies will have been published, completing the annual assessment cycle.</t>
-  </si>
-  <si>
     <t>AG</t>
   </si>
   <si>
@@ -536,15 +584,17 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">*Note that TPI has only started disclosing company's alignment in 2025 and 2035 in 2022 hence </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>this column should be blank as of March 2022</t>
     </r>
@@ -561,15 +611,17 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">*Note that TPI has only started disclosing company's alignment in 2027 in 2024 hence </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>this column should be blank as of January 2022</t>
     </r>
@@ -607,15 +659,17 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">*Note that TPI has only started disclosing company's years with targets in 2022 hence </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>this column should be blank as of March 2022</t>
     </r>
@@ -730,28 +784,21 @@
   </si>
   <si>
     <t>Carbon intensity values for each year of the benchmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date on which the company's Carbon Performance assessment was conducted (companies are assessed annually). Some of the companies that the TPI assesses also include companies from the CA100+. Please note that from 2024, the Carbon Performance (CP) data for the TPI companies which are not part of the CA100+ universe are released earlier in a given year, rather than in the autumn, which is typically when CA100+ company assessments are published. Therefore, ‘non-CA100+’ companies within each sector may display more up-to-date publication dates until the third quarter (Q3) of a calendar year. By Q3, data for all companies, including CA100+ companies, will have been published, completing the annual assessment cycle. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date on which the company's Carbon Performance assessment was conducted (companies are assessed annually). Please note that from 2024, the Carbon Performance (CP) data for the TPI companies which are not part of the CA100+ universe are released earlier in a given year, rather than in the autumn, which is typically when CA100+ company assessments are published. Therefore, ‘non-CA100+’ companies within each sector may display more up-to-date publication dates until the third quarter (Q3) of a calendar year. By Q3, data for all companies, including CA100+ companies, will have been published, completing the annual assessment cycle. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -759,25 +806,35 @@
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1063,94 +1120,70 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="26">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1160,26 +1193,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffe1ff"/>
-      <rgbColor rgb="ffb4c6e7"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFFFE1FF"/>
+      <rgbColor rgb="FFB4C6E7"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -1381,7 +1473,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1399,7 +1491,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1428,7 +1520,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1453,7 +1545,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1478,7 +1570,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1503,7 +1595,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1528,7 +1620,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1553,7 +1645,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1578,7 +1670,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1603,7 +1695,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1628,7 +1720,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1641,9 +1733,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1660,7 +1758,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1678,7 +1776,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1703,7 +1801,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1728,7 +1826,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1753,7 +1851,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1778,7 +1876,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1803,7 +1901,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1828,7 +1926,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1853,7 +1951,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1878,7 +1976,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1903,7 +2001,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1916,9 +2014,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1932,7 +2036,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1950,7 +2054,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1979,7 +2083,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2004,7 +2108,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2029,7 +2133,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2054,7 +2158,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2079,7 +2183,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2104,7 +2208,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2129,7 +2233,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2154,7 +2258,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2179,7 +2283,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2192,35 +2296,44 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU34"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="2" width="8.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="43" style="1" customWidth="1"/>
-    <col min="4" max="4" width="96.1719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="72.1719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="79.1719" style="1" customWidth="1"/>
-    <col min="8" max="47" width="8.85156" style="1" customWidth="1"/>
-    <col min="48" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="4" max="4" width="96.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="72.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="79.21875" style="1" customWidth="1"/>
+    <col min="8" max="48" width="8.88671875" style="1" customWidth="1"/>
+    <col min="49" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2269,17 +2382,17 @@
       <c r="AT1" s="2"/>
       <c r="AU1" s="2"/>
     </row>
-    <row r="2" ht="400.8" customHeight="1">
+    <row r="2" spans="1:47" ht="400.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -2320,14 +2433,14 @@
       <c r="AT2" s="2"/>
       <c r="AU2" s="2"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -2369,27 +2482,27 @@
       <c r="AT3" s="2"/>
       <c r="AU3" s="2"/>
     </row>
-    <row r="4" ht="14.05" customHeight="1">
+    <row r="4" spans="1:47" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
-      <c r="B4" t="s" s="10">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F4" t="s" s="11">
+      <c r="F4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G4" t="s" s="12">
+      <c r="G4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -2430,23 +2543,23 @@
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
+    <row r="5" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
-      <c r="B5" t="s" s="13">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s" s="14">
+      <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s" s="15">
+      <c r="D5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" t="s" s="15">
+      <c r="E5" s="13"/>
+      <c r="F5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="8"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2487,23 +2600,23 @@
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
     </row>
-    <row r="6" ht="28.8" customHeight="1">
+    <row r="6" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" t="s" s="13">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s" s="14">
+      <c r="C6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="15">
+      <c r="D6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" t="s" s="15">
+      <c r="E6" s="13"/>
+      <c r="F6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -2544,23 +2657,23 @@
       <c r="AT6" s="2"/>
       <c r="AU6" s="2"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
+    <row r="7" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" t="s" s="13">
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s" s="14">
+      <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s" s="15">
+      <c r="D7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" t="s" s="15">
+      <c r="E7" s="13"/>
+      <c r="F7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -2601,23 +2714,23 @@
       <c r="AT7" s="2"/>
       <c r="AU7" s="2"/>
     </row>
-    <row r="8" ht="57.6" customHeight="1">
+    <row r="8" spans="1:47" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" t="s" s="13">
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s" s="14">
+      <c r="C8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s" s="15">
+      <c r="D8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" t="s" s="15">
+      <c r="E8" s="13"/>
+      <c r="F8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -2658,25 +2771,25 @@
       <c r="AT8" s="2"/>
       <c r="AU8" s="2"/>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
+    <row r="9" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
-      <c r="B9" t="s" s="13">
+      <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s" s="14">
+      <c r="C9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s" s="15">
+      <c r="D9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s" s="15">
+      <c r="E9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F9" t="s" s="15">
+      <c r="F9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -2717,25 +2830,25 @@
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
     </row>
-    <row r="10" ht="13.55" customHeight="1">
+    <row r="10" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" t="s" s="13">
+      <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s" s="14">
+      <c r="C10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s" s="15">
+      <c r="D10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s" s="15">
+      <c r="E10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F10" t="s" s="15">
+      <c r="F10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -2776,23 +2889,23 @@
       <c r="AT10" s="2"/>
       <c r="AU10" s="2"/>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
+    <row r="11" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
-      <c r="B11" t="s" s="13">
+      <c r="B11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s" s="14">
+      <c r="C11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s" s="15">
+      <c r="D11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" t="s" s="15">
+      <c r="E11" s="13"/>
+      <c r="F11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -2833,25 +2946,25 @@
       <c r="AT11" s="2"/>
       <c r="AU11" s="2"/>
     </row>
-    <row r="12" ht="13.55" customHeight="1">
+    <row r="12" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
-      <c r="B12" t="s" s="13">
+      <c r="B12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s" s="14">
+      <c r="C12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s" s="15">
+      <c r="D12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E12" t="s" s="15">
+      <c r="E12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F12" t="s" s="15">
+      <c r="F12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="8"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -2892,25 +3005,25 @@
       <c r="AT12" s="2"/>
       <c r="AU12" s="2"/>
     </row>
-    <row r="13" ht="28.8" customHeight="1">
+    <row r="13" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
-      <c r="B13" t="s" s="13">
+      <c r="B13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s" s="14">
+      <c r="C13" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s" s="15">
+      <c r="D13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E13" t="s" s="15">
+      <c r="E13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F13" t="s" s="15">
+      <c r="F13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="8"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="5"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -2951,25 +3064,25 @@
       <c r="AT13" s="2"/>
       <c r="AU13" s="2"/>
     </row>
-    <row r="14" ht="28.8" customHeight="1">
+    <row r="14" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
-      <c r="B14" t="s" s="13">
+      <c r="B14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s" s="14">
+      <c r="C14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D14" t="s" s="15">
+      <c r="D14" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E14" t="s" s="15">
+      <c r="E14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F14" t="s" s="15">
+      <c r="F14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -3008,29 +3121,29 @@
       <c r="AR14" s="2"/>
       <c r="AS14" s="2"/>
       <c r="AT14" s="2"/>
-      <c r="AU14" t="s" s="18">
+      <c r="AU14" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" ht="13.55" customHeight="1">
+    <row r="15" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
-      <c r="B15" t="s" s="13">
+      <c r="B15" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s" s="14">
+      <c r="C15" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D15" t="s" s="15">
+      <c r="D15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E15" t="s" s="15">
+      <c r="E15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F15" t="s" s="15">
+      <c r="F15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="8"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -3071,25 +3184,25 @@
       <c r="AT15" s="2"/>
       <c r="AU15" s="2"/>
     </row>
-    <row r="16" ht="28.8" customHeight="1">
+    <row r="16" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
-      <c r="B16" t="s" s="13">
+      <c r="B16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C16" t="s" s="14">
+      <c r="C16" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D16" t="s" s="15">
+      <c r="D16" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E16" t="s" s="15">
+      <c r="E16" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F16" t="s" s="15">
+      <c r="F16" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="8"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -3130,25 +3243,25 @@
       <c r="AT16" s="2"/>
       <c r="AU16" s="2"/>
     </row>
-    <row r="17" ht="13.55" customHeight="1">
+    <row r="17" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
-      <c r="B17" t="s" s="13">
+      <c r="B17" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C17" t="s" s="14">
+      <c r="C17" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D17" t="s" s="15">
+      <c r="D17" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E17" t="s" s="15">
+      <c r="E17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F17" t="s" s="15">
+      <c r="F17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="8"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="5"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -3189,25 +3302,25 @@
       <c r="AT17" s="2"/>
       <c r="AU17" s="2"/>
     </row>
-    <row r="18" ht="71.05" customHeight="1">
+    <row r="18" spans="1:47" ht="138" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
-      <c r="B18" t="s" s="13">
+      <c r="B18" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C18" t="s" s="14">
+      <c r="C18" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D18" t="s" s="15">
-        <v>57</v>
-      </c>
-      <c r="E18" t="s" s="15">
+      <c r="D18" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F18" t="s" s="15">
+      <c r="F18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="8"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -3248,25 +3361,25 @@
       <c r="AT18" s="2"/>
       <c r="AU18" s="2"/>
     </row>
-    <row r="19" ht="13.55" customHeight="1">
+    <row r="19" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
-      <c r="B19" t="s" s="13">
+      <c r="B19" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C19" t="s" s="14">
+      <c r="D19" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D19" t="s" s="15">
-        <v>60</v>
-      </c>
-      <c r="E19" t="s" s="15">
+      <c r="E19" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F19" t="s" s="15">
+      <c r="F19" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="8"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="5"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -3307,23 +3420,23 @@
       <c r="AT19" s="2"/>
       <c r="AU19" s="2"/>
     </row>
-    <row r="20" ht="28.8" customHeight="1">
+    <row r="20" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
-      <c r="B20" t="s" s="13">
+      <c r="B20" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C20" t="s" s="14">
+      <c r="D20" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D20" t="s" s="15">
-        <v>63</v>
-      </c>
-      <c r="E20" s="16"/>
-      <c r="F20" t="s" s="15">
+      <c r="E20" s="13"/>
+      <c r="F20" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="8"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -3364,27 +3477,27 @@
       <c r="AT20" s="2"/>
       <c r="AU20" s="2"/>
     </row>
-    <row r="21" ht="28.8" customHeight="1">
+    <row r="21" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
-      <c r="B21" t="s" s="13">
+      <c r="B21" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C21" t="s" s="14">
+      <c r="D21" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D21" t="s" s="15">
+      <c r="E21" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E21" t="s" s="15">
+      <c r="F21" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F21" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="G21" t="s" s="19">
-        <v>68</v>
-      </c>
-      <c r="H21" s="8"/>
+      <c r="H21" s="5"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -3425,27 +3538,27 @@
       <c r="AT21" s="2"/>
       <c r="AU21" s="2"/>
     </row>
-    <row r="22" ht="28.8" customHeight="1">
+    <row r="22" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
-      <c r="B22" t="s" s="13">
-        <v>64</v>
-      </c>
-      <c r="C22" t="s" s="14">
+      <c r="B22" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D22" t="s" s="15">
-        <v>70</v>
-      </c>
-      <c r="E22" t="s" s="15">
+      <c r="E22" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F22" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="G22" t="s" s="19">
-        <v>68</v>
-      </c>
-      <c r="H22" s="8"/>
+      <c r="H22" s="5"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -3486,27 +3599,27 @@
       <c r="AT22" s="2"/>
       <c r="AU22" s="2"/>
     </row>
-    <row r="23" ht="28.8" customHeight="1">
+    <row r="23" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
-      <c r="B23" t="s" s="13">
+      <c r="B23" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C23" t="s" s="14">
+      <c r="D23" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D23" t="s" s="15">
-        <v>73</v>
-      </c>
-      <c r="E23" t="s" s="15">
+      <c r="E23" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F23" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="G23" t="s" s="19">
-        <v>68</v>
-      </c>
-      <c r="H23" s="8"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -3547,27 +3660,27 @@
       <c r="AT23" s="2"/>
       <c r="AU23" s="2"/>
     </row>
-    <row r="24" ht="28.8" customHeight="1">
+    <row r="24" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
-      <c r="B24" t="s" s="13">
+      <c r="B24" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C24" t="s" s="14">
+      <c r="D24" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D24" t="s" s="15">
-        <v>76</v>
-      </c>
-      <c r="E24" t="s" s="15">
+      <c r="E24" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F24" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="G24" t="s" s="19">
-        <v>68</v>
-      </c>
-      <c r="H24" s="8"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -3608,23 +3721,23 @@
       <c r="AT24" s="2"/>
       <c r="AU24" s="2"/>
     </row>
-    <row r="25" ht="13.55" customHeight="1">
+    <row r="25" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
-      <c r="B25" t="s" s="13">
+      <c r="B25" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C25" t="s" s="14">
+      <c r="D25" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D25" t="s" s="15">
-        <v>79</v>
-      </c>
-      <c r="E25" s="16"/>
-      <c r="F25" t="s" s="15">
+      <c r="E25" s="13"/>
+      <c r="F25" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="8"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="5"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -3665,25 +3778,25 @@
       <c r="AT25" s="2"/>
       <c r="AU25" s="2"/>
     </row>
-    <row r="26" ht="28.8" customHeight="1">
+    <row r="26" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
-      <c r="B26" t="s" s="13">
+      <c r="B26" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C26" t="s" s="14">
+      <c r="D26" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D26" t="s" s="15">
+      <c r="E26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E26" t="s" s="15">
-        <v>83</v>
-      </c>
-      <c r="F26" t="s" s="15">
+      <c r="F26" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="8"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="5"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -3724,25 +3837,25 @@
       <c r="AT26" s="2"/>
       <c r="AU26" s="2"/>
     </row>
-    <row r="27" ht="28.8" customHeight="1">
+    <row r="27" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
-      <c r="B27" t="s" s="13">
-        <v>80</v>
-      </c>
-      <c r="C27" t="s" s="14">
+      <c r="B27" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D27" t="s" s="15">
+      <c r="E27" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E27" t="s" s="15">
-        <v>86</v>
-      </c>
-      <c r="F27" t="s" s="15">
+      <c r="F27" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="8"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="5"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -3783,25 +3896,25 @@
       <c r="AT27" s="2"/>
       <c r="AU27" s="2"/>
     </row>
-    <row r="28" ht="28.8" customHeight="1">
+    <row r="28" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
-      <c r="B28" t="s" s="13">
+      <c r="B28" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C28" t="s" s="14">
+      <c r="D28" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D28" t="s" s="15">
-        <v>89</v>
-      </c>
-      <c r="E28" t="s" s="15">
-        <v>83</v>
-      </c>
-      <c r="F28" t="s" s="15">
+      <c r="E28" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="8"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="5"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -3842,23 +3955,23 @@
       <c r="AT28" s="2"/>
       <c r="AU28" s="2"/>
     </row>
-    <row r="29" ht="28.8" customHeight="1">
+    <row r="29" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
-      <c r="B29" t="s" s="13">
+      <c r="B29" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C29" t="s" s="14">
+      <c r="D29" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D29" t="s" s="15">
-        <v>92</v>
-      </c>
-      <c r="E29" s="16"/>
-      <c r="F29" t="s" s="15">
+      <c r="E29" s="13"/>
+      <c r="F29" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="8"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="5"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -3899,25 +4012,25 @@
       <c r="AT29" s="2"/>
       <c r="AU29" s="2"/>
     </row>
-    <row r="30" ht="28.8" customHeight="1">
+    <row r="30" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
-      <c r="B30" t="s" s="13">
+      <c r="B30" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C30" t="s" s="14">
+      <c r="D30" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D30" t="s" s="15">
+      <c r="E30" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E30" t="s" s="15">
-        <v>96</v>
-      </c>
-      <c r="F30" t="s" s="15">
+      <c r="F30" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="8"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="5"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -3958,23 +4071,23 @@
       <c r="AT30" s="2"/>
       <c r="AU30" s="2"/>
     </row>
-    <row r="31" ht="28.8" customHeight="1">
+    <row r="31" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
-      <c r="B31" t="s" s="13">
+      <c r="B31" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C31" t="s" s="14">
+      <c r="D31" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D31" t="s" s="15">
-        <v>99</v>
-      </c>
-      <c r="E31" s="16"/>
-      <c r="F31" t="s" s="15">
+      <c r="E31" s="13"/>
+      <c r="F31" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G31" s="17"/>
-      <c r="H31" s="8"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="5"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -4015,23 +4128,23 @@
       <c r="AT31" s="2"/>
       <c r="AU31" s="2"/>
     </row>
-    <row r="32" ht="13.55" customHeight="1">
+    <row r="32" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
-      <c r="B32" t="s" s="13">
+      <c r="B32" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C32" t="s" s="14">
+      <c r="D32" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D32" t="s" s="15">
-        <v>102</v>
-      </c>
-      <c r="E32" s="16"/>
-      <c r="F32" t="s" s="15">
+      <c r="E32" s="13"/>
+      <c r="F32" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="17"/>
-      <c r="H32" s="8"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="5"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -4072,23 +4185,23 @@
       <c r="AT32" s="2"/>
       <c r="AU32" s="2"/>
     </row>
-    <row r="33" ht="28.8" customHeight="1">
+    <row r="33" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
-      <c r="B33" t="s" s="13">
+      <c r="B33" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C33" t="s" s="14">
+      <c r="D33" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D33" t="s" s="15">
+      <c r="E33" s="13"/>
+      <c r="F33" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="16"/>
-      <c r="F33" t="s" s="15">
-        <v>106</v>
-      </c>
-      <c r="G33" s="17"/>
-      <c r="H33" s="8"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="5"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
@@ -4129,23 +4242,23 @@
       <c r="AT33" s="2"/>
       <c r="AU33" s="2"/>
     </row>
-    <row r="34" ht="31.5" customHeight="1">
+    <row r="34" spans="1:47" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
-      <c r="B34" t="s" s="20">
+      <c r="B34" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C34" t="s" s="21">
+      <c r="D34" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="D34" t="s" s="22">
-        <v>109</v>
-      </c>
-      <c r="E34" s="23"/>
-      <c r="F34" t="s" s="22">
+      <c r="E34" s="20"/>
+      <c r="F34" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="24"/>
-      <c r="H34" s="8"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="5"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -4191,7 +4304,7 @@
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -4199,24 +4312,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85156" style="25" customWidth="1"/>
-    <col min="3" max="3" width="43" style="25" customWidth="1"/>
-    <col min="4" max="4" width="96.1719" style="25" customWidth="1"/>
-    <col min="5" max="5" width="72.1719" style="25" customWidth="1"/>
-    <col min="6" max="6" width="16.8516" style="25" customWidth="1"/>
-    <col min="7" max="7" width="78.8516" style="25" customWidth="1"/>
-    <col min="8" max="47" width="8.85156" style="25" customWidth="1"/>
-    <col min="48" max="16384" width="8.85156" style="25" customWidth="1"/>
+    <col min="1" max="2" width="8.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43" style="1" customWidth="1"/>
+    <col min="4" max="4" width="96.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="72.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="78.88671875" style="1" customWidth="1"/>
+    <col min="8" max="48" width="8.88671875" style="1" customWidth="1"/>
+    <col min="49" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4265,17 +4380,17 @@
       <c r="AT1" s="2"/>
       <c r="AU1" s="2"/>
     </row>
-    <row r="2" ht="381" customHeight="1">
+    <row r="2" spans="1:47" ht="381" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -4316,14 +4431,14 @@
       <c r="AT2" s="2"/>
       <c r="AU2" s="2"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -4365,27 +4480,27 @@
       <c r="AT3" s="2"/>
       <c r="AU3" s="2"/>
     </row>
-    <row r="4" ht="14.05" customHeight="1">
+    <row r="4" spans="1:47" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
-      <c r="B4" t="s" s="10">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F4" t="s" s="11">
+      <c r="F4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G4" t="s" s="12">
+      <c r="G4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -4426,23 +4541,23 @@
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
+    <row r="5" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
-      <c r="B5" t="s" s="13">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s" s="14">
+      <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s" s="15">
+      <c r="D5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" t="s" s="15">
+      <c r="E5" s="13"/>
+      <c r="F5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="8"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -4483,23 +4598,23 @@
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
     </row>
-    <row r="6" ht="28.8" customHeight="1">
+    <row r="6" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" t="s" s="13">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s" s="14">
+      <c r="C6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="15">
+      <c r="D6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" t="s" s="15">
+      <c r="E6" s="13"/>
+      <c r="F6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -4540,23 +4655,23 @@
       <c r="AT6" s="2"/>
       <c r="AU6" s="2"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
+    <row r="7" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" t="s" s="13">
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s" s="14">
+      <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s" s="15">
+      <c r="D7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" t="s" s="15">
+      <c r="E7" s="13"/>
+      <c r="F7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -4597,23 +4712,23 @@
       <c r="AT7" s="2"/>
       <c r="AU7" s="2"/>
     </row>
-    <row r="8" ht="57.6" customHeight="1">
+    <row r="8" spans="1:47" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" t="s" s="13">
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s" s="14">
+      <c r="C8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s" s="15">
+      <c r="D8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" t="s" s="15">
+      <c r="E8" s="13"/>
+      <c r="F8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -4654,25 +4769,25 @@
       <c r="AT8" s="2"/>
       <c r="AU8" s="2"/>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
+    <row r="9" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
-      <c r="B9" t="s" s="13">
+      <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s" s="14">
+      <c r="C9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s" s="15">
+      <c r="D9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s" s="15">
+      <c r="E9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F9" t="s" s="15">
+      <c r="F9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -4713,25 +4828,25 @@
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
     </row>
-    <row r="10" ht="13.55" customHeight="1">
+    <row r="10" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" t="s" s="13">
+      <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s" s="14">
+      <c r="C10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s" s="15">
+      <c r="D10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s" s="15">
+      <c r="E10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F10" t="s" s="15">
+      <c r="F10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -4772,23 +4887,23 @@
       <c r="AT10" s="2"/>
       <c r="AU10" s="2"/>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
+    <row r="11" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
-      <c r="B11" t="s" s="13">
+      <c r="B11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s" s="14">
+      <c r="C11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s" s="15">
+      <c r="D11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" t="s" s="15">
+      <c r="E11" s="13"/>
+      <c r="F11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -4829,25 +4944,25 @@
       <c r="AT11" s="2"/>
       <c r="AU11" s="2"/>
     </row>
-    <row r="12" ht="13.55" customHeight="1">
+    <row r="12" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
-      <c r="B12" t="s" s="13">
+      <c r="B12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s" s="14">
+      <c r="C12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s" s="15">
+      <c r="D12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E12" t="s" s="15">
+      <c r="E12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F12" t="s" s="15">
+      <c r="F12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="8"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -4888,25 +5003,25 @@
       <c r="AT12" s="2"/>
       <c r="AU12" s="2"/>
     </row>
-    <row r="13" ht="65.55" customHeight="1">
+    <row r="13" spans="1:47" ht="65.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
-      <c r="B13" t="s" s="13">
+      <c r="B13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s" s="14">
-        <v>110</v>
-      </c>
-      <c r="D13" t="s" s="15">
-        <v>57</v>
-      </c>
-      <c r="E13" t="s" s="15">
+      <c r="C13" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F13" t="s" s="15">
+      <c r="F13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="8"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="5"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -4947,25 +5062,25 @@
       <c r="AT13" s="2"/>
       <c r="AU13" s="2"/>
     </row>
-    <row r="14" ht="13.55" customHeight="1">
+    <row r="14" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
-      <c r="B14" t="s" s="13">
+      <c r="B14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s" s="14">
-        <v>111</v>
-      </c>
-      <c r="D14" t="s" s="15">
-        <v>60</v>
-      </c>
-      <c r="E14" t="s" s="15">
+      <c r="C14" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F14" t="s" s="15">
+      <c r="F14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -5004,31 +5119,31 @@
       <c r="AR14" s="2"/>
       <c r="AS14" s="2"/>
       <c r="AT14" s="2"/>
-      <c r="AU14" t="s" s="18">
+      <c r="AU14" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" ht="28.8" customHeight="1">
+    <row r="15" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
-      <c r="B15" t="s" s="13">
+      <c r="B15" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s" s="14">
+      <c r="C15" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D15" t="s" s="15">
+      <c r="E15" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E15" t="s" s="15">
+      <c r="F15" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F15" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="G15" t="s" s="19">
-        <v>68</v>
-      </c>
-      <c r="H15" s="8"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -5069,27 +5184,27 @@
       <c r="AT15" s="2"/>
       <c r="AU15" s="2"/>
     </row>
-    <row r="16" ht="28.8" customHeight="1">
+    <row r="16" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
-      <c r="B16" t="s" s="13">
+      <c r="B16" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C16" t="s" s="14">
+      <c r="C16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D16" t="s" s="15">
-        <v>70</v>
-      </c>
-      <c r="E16" t="s" s="15">
+      <c r="E16" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F16" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="G16" t="s" s="19">
-        <v>68</v>
-      </c>
-      <c r="H16" s="8"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -5130,27 +5245,27 @@
       <c r="AT16" s="2"/>
       <c r="AU16" s="2"/>
     </row>
-    <row r="17" ht="28.8" customHeight="1">
+    <row r="17" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
-      <c r="B17" t="s" s="13">
+      <c r="B17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C17" t="s" s="14">
+      <c r="C17" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D17" t="s" s="15">
-        <v>73</v>
-      </c>
-      <c r="E17" t="s" s="15">
+      <c r="E17" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F17" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="G17" t="s" s="19">
-        <v>68</v>
-      </c>
-      <c r="H17" s="8"/>
+      <c r="H17" s="5"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -5191,27 +5306,27 @@
       <c r="AT17" s="2"/>
       <c r="AU17" s="2"/>
     </row>
-    <row r="18" ht="28.8" customHeight="1">
+    <row r="18" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
-      <c r="B18" t="s" s="13">
-        <v>112</v>
-      </c>
-      <c r="C18" t="s" s="14">
+      <c r="B18" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D18" t="s" s="15">
-        <v>76</v>
-      </c>
-      <c r="E18" t="s" s="15">
+      <c r="E18" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F18" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="G18" t="s" s="19">
-        <v>68</v>
-      </c>
-      <c r="H18" s="8"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -5252,23 +5367,23 @@
       <c r="AT18" s="2"/>
       <c r="AU18" s="2"/>
     </row>
-    <row r="19" ht="13.55" customHeight="1">
+    <row r="19" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
-      <c r="B19" t="s" s="13">
-        <v>113</v>
-      </c>
-      <c r="C19" t="s" s="14">
+      <c r="B19" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D19" t="s" s="15">
-        <v>79</v>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" t="s" s="15">
+      <c r="E19" s="13"/>
+      <c r="F19" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="8"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="5"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -5309,23 +5424,23 @@
       <c r="AT19" s="2"/>
       <c r="AU19" s="2"/>
     </row>
-    <row r="20" ht="28.8" customHeight="1">
+    <row r="20" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
-      <c r="B20" t="s" s="13">
-        <v>114</v>
-      </c>
-      <c r="C20" t="s" s="14">
+      <c r="B20" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D20" t="s" s="15">
-        <v>63</v>
-      </c>
-      <c r="E20" s="16"/>
-      <c r="F20" t="s" s="15">
+      <c r="E20" s="13"/>
+      <c r="F20" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="8"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -5366,23 +5481,23 @@
       <c r="AT20" s="2"/>
       <c r="AU20" s="2"/>
     </row>
-    <row r="21" ht="28.8" customHeight="1">
+    <row r="21" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
-      <c r="B21" t="s" s="13">
+      <c r="B21" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C21" t="s" s="14">
-        <v>116</v>
-      </c>
-      <c r="D21" t="s" s="15">
-        <v>99</v>
-      </c>
-      <c r="E21" s="16"/>
-      <c r="F21" t="s" s="15">
+      <c r="D21" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="8"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="5"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -5423,23 +5538,23 @@
       <c r="AT21" s="2"/>
       <c r="AU21" s="2"/>
     </row>
-    <row r="22" ht="13.55" customHeight="1">
+    <row r="22" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
-      <c r="B22" t="s" s="13">
-        <v>117</v>
-      </c>
-      <c r="C22" t="s" s="14">
+      <c r="B22" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D22" t="s" s="15">
-        <v>102</v>
-      </c>
-      <c r="E22" s="16"/>
-      <c r="F22" t="s" s="15">
+      <c r="D22" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="8"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="5"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -5480,23 +5595,23 @@
       <c r="AT22" s="2"/>
       <c r="AU22" s="2"/>
     </row>
-    <row r="23" ht="13.55" customHeight="1">
+    <row r="23" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
-      <c r="B23" t="s" s="13">
-        <v>118</v>
-      </c>
-      <c r="C23" t="s" s="14">
+      <c r="B23" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="D23" t="s" s="15">
-        <v>109</v>
-      </c>
-      <c r="E23" s="16"/>
-      <c r="F23" t="s" s="15">
+      <c r="E23" s="13"/>
+      <c r="F23" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="8"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -5537,23 +5652,23 @@
       <c r="AT23" s="2"/>
       <c r="AU23" s="2"/>
     </row>
-    <row r="24" ht="29.4" customHeight="1">
+    <row r="24" spans="1:47" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
-      <c r="B24" t="s" s="20">
-        <v>119</v>
-      </c>
-      <c r="C24" t="s" s="21">
+      <c r="B24" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D24" t="s" s="22">
+      <c r="E24" s="20"/>
+      <c r="F24" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="23"/>
-      <c r="F24" t="s" s="22">
-        <v>106</v>
-      </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="8"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -5599,7 +5714,7 @@
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -5607,24 +5722,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AU17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85156" style="26" customWidth="1"/>
-    <col min="3" max="3" width="43" style="26" customWidth="1"/>
-    <col min="4" max="4" width="96.1719" style="26" customWidth="1"/>
-    <col min="5" max="5" width="72.1719" style="26" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="26" customWidth="1"/>
-    <col min="7" max="7" width="76.5" style="26" customWidth="1"/>
-    <col min="8" max="47" width="8.85156" style="26" customWidth="1"/>
-    <col min="48" max="16384" width="8.85156" style="26" customWidth="1"/>
+    <col min="1" max="2" width="8.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43" style="1" customWidth="1"/>
+    <col min="4" max="4" width="96.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="72.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="76.44140625" style="1" customWidth="1"/>
+    <col min="8" max="48" width="8.88671875" style="1" customWidth="1"/>
+    <col min="49" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5673,17 +5788,17 @@
       <c r="AT1" s="2"/>
       <c r="AU1" s="2"/>
     </row>
-    <row r="2" ht="406.2" customHeight="1">
+    <row r="2" spans="1:47" ht="406.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -5724,14 +5839,14 @@
       <c r="AT2" s="2"/>
       <c r="AU2" s="2"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
+    <row r="3" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -5773,27 +5888,27 @@
       <c r="AT3" s="2"/>
       <c r="AU3" s="2"/>
     </row>
-    <row r="4" ht="14.05" customHeight="1">
+    <row r="4" spans="1:47" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
-      <c r="B4" t="s" s="10">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F4" t="s" s="11">
+      <c r="F4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G4" t="s" s="12">
+      <c r="G4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -5834,23 +5949,23 @@
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
+    <row r="5" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
-      <c r="B5" t="s" s="13">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s" s="14">
+      <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s" s="15">
+      <c r="D5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" t="s" s="15">
+      <c r="E5" s="13"/>
+      <c r="F5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="8"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -5891,23 +6006,23 @@
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
     </row>
-    <row r="6" ht="28.8" customHeight="1">
+    <row r="6" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" t="s" s="13">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s" s="14">
+      <c r="C6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="15">
+      <c r="D6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" t="s" s="15">
+      <c r="E6" s="13"/>
+      <c r="F6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -5948,23 +6063,23 @@
       <c r="AT6" s="2"/>
       <c r="AU6" s="2"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
+    <row r="7" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" t="s" s="13">
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s" s="14">
+      <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s" s="15">
+      <c r="D7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" t="s" s="15">
+      <c r="E7" s="13"/>
+      <c r="F7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -6005,23 +6120,23 @@
       <c r="AT7" s="2"/>
       <c r="AU7" s="2"/>
     </row>
-    <row r="8" ht="57.6" customHeight="1">
+    <row r="8" spans="1:47" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" t="s" s="13">
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s" s="14">
+      <c r="C8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s" s="15">
+      <c r="D8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" t="s" s="15">
+      <c r="E8" s="13"/>
+      <c r="F8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -6062,25 +6177,25 @@
       <c r="AT8" s="2"/>
       <c r="AU8" s="2"/>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
+    <row r="9" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
-      <c r="B9" t="s" s="13">
+      <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s" s="14">
-        <v>120</v>
-      </c>
-      <c r="D9" t="s" s="15">
+      <c r="C9" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s" s="15">
+      <c r="E9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F9" t="s" s="15">
+      <c r="F9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -6121,25 +6236,25 @@
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
     </row>
-    <row r="10" ht="13.55" customHeight="1">
+    <row r="10" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" t="s" s="13">
+      <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s" s="14">
+      <c r="C10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s" s="15">
+      <c r="D10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s" s="15">
+      <c r="E10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F10" t="s" s="15">
+      <c r="F10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -6180,23 +6295,23 @@
       <c r="AT10" s="2"/>
       <c r="AU10" s="2"/>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
+    <row r="11" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
-      <c r="B11" t="s" s="13">
+      <c r="B11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s" s="14">
+      <c r="C11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s" s="15">
+      <c r="D11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" t="s" s="15">
+      <c r="E11" s="13"/>
+      <c r="F11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -6237,25 +6352,25 @@
       <c r="AT11" s="2"/>
       <c r="AU11" s="2"/>
     </row>
-    <row r="12" ht="13.55" customHeight="1">
+    <row r="12" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
-      <c r="B12" t="s" s="13">
+      <c r="B12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s" s="14">
+      <c r="C12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s" s="15">
+      <c r="D12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E12" t="s" s="15">
+      <c r="E12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F12" t="s" s="15">
+      <c r="F12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="8"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -6296,25 +6411,25 @@
       <c r="AT12" s="2"/>
       <c r="AU12" s="2"/>
     </row>
-    <row r="13" ht="28.8" customHeight="1">
+    <row r="13" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
-      <c r="B13" t="s" s="13">
+      <c r="B13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s" s="14">
-        <v>110</v>
-      </c>
-      <c r="D13" t="s" s="15">
+      <c r="C13" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E13" t="s" s="15">
+      <c r="E13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F13" t="s" s="15">
+      <c r="F13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="8"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="5"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -6355,25 +6470,25 @@
       <c r="AT13" s="2"/>
       <c r="AU13" s="2"/>
     </row>
-    <row r="14" ht="28.8" customHeight="1">
+    <row r="14" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
-      <c r="B14" t="s" s="13">
+      <c r="B14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s" s="14">
-        <v>111</v>
-      </c>
-      <c r="D14" t="s" s="15">
+      <c r="C14" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E14" t="s" s="15">
+      <c r="E14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F14" t="s" s="15">
+      <c r="F14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -6412,29 +6527,29 @@
       <c r="AR14" s="2"/>
       <c r="AS14" s="2"/>
       <c r="AT14" s="2"/>
-      <c r="AU14" t="s" s="18">
+      <c r="AU14" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" ht="13.55" customHeight="1">
+    <row r="15" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
-      <c r="B15" t="s" s="13">
+      <c r="B15" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s" s="14">
+      <c r="C15" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D15" t="s" s="15">
+      <c r="D15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E15" t="s" s="15">
+      <c r="E15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F15" t="s" s="15">
+      <c r="F15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="8"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -6475,25 +6590,25 @@
       <c r="AT15" s="2"/>
       <c r="AU15" s="2"/>
     </row>
-    <row r="16" ht="28.8" customHeight="1">
+    <row r="16" spans="1:47" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
-      <c r="B16" t="s" s="13">
+      <c r="B16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C16" t="s" s="14">
-        <v>121</v>
-      </c>
-      <c r="D16" t="s" s="15">
+      <c r="C16" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E16" t="s" s="15">
+      <c r="E16" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F16" t="s" s="15">
+      <c r="F16" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="8"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -6534,25 +6649,25 @@
       <c r="AT16" s="2"/>
       <c r="AU16" s="2"/>
     </row>
-    <row r="17" ht="34.05" customHeight="1">
+    <row r="17" spans="1:47" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
-      <c r="B17" t="s" s="20">
+      <c r="B17" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C17" t="s" s="21">
+      <c r="C17" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D17" t="s" s="22">
-        <v>53</v>
-      </c>
-      <c r="E17" t="s" s="22">
-        <v>123</v>
-      </c>
-      <c r="F17" t="s" s="22">
+      <c r="F17" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="8"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="5"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -6598,7 +6713,7 @@
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -6606,23 +6721,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.85156" style="27" customWidth="1"/>
-    <col min="3" max="3" width="43" style="27" customWidth="1"/>
-    <col min="4" max="4" width="96.1719" style="27" customWidth="1"/>
-    <col min="5" max="5" width="72.1719" style="27" customWidth="1"/>
-    <col min="6" max="6" width="16.1719" style="27" customWidth="1"/>
-    <col min="7" max="7" width="78.8516" style="27" customWidth="1"/>
-    <col min="8" max="16384" width="8.85156" style="27" customWidth="1"/>
+    <col min="1" max="2" width="8.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43" style="1" customWidth="1"/>
+    <col min="4" max="4" width="96.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="72.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="78.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6631,163 +6747,163 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" ht="381" customHeight="1">
+    <row r="2" spans="1:7" ht="381" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" ht="14.05" customHeight="1">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
-      <c r="B4" t="s" s="10">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F4" t="s" s="11">
+      <c r="F4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G4" t="s" s="12">
+      <c r="G4" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="28.8" customHeight="1">
+    <row r="5" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
-      <c r="B5" t="s" s="13">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s" s="14">
+      <c r="C5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D5" t="s" s="15">
-        <v>63</v>
-      </c>
-      <c r="E5" t="s" s="15">
+      <c r="E5" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F5" t="s" s="15">
+      <c r="D6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6" ht="57.6" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" t="s" s="13">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s" s="14">
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D6" t="s" s="15">
-        <v>18</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" t="s" s="15">
+      <c r="D7" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" ht="28.8" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" t="s" s="13">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s" s="14">
-        <v>126</v>
-      </c>
-      <c r="D7" t="s" s="15">
-        <v>127</v>
-      </c>
-      <c r="E7" t="s" s="15">
+      <c r="G7" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="F7" t="s" s="15">
+      <c r="D8" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G7" t="s" s="19">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" t="s" s="13">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s" s="14">
-        <v>129</v>
-      </c>
-      <c r="D8" t="s" s="15">
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E8" t="s" s="15">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s" s="15">
+      <c r="D9" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" t="s" s="13">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s" s="14">
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="D9" t="s" s="15">
-        <v>102</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="G9" s="17"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" t="s" s="20">
+      <c r="C10" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C10" t="s" s="21">
-        <v>104</v>
-      </c>
-      <c r="D10" t="s" s="22">
-        <v>133</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="F10" t="s" s="22">
-        <v>106</v>
-      </c>
-      <c r="G10" s="24"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>